<commit_message>
Added Results and Comments Entry in Excel File
</commit_message>
<xml_diff>
--- a/LeadFiles/leads.xlsx
+++ b/LeadFiles/leads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Training Courses\RPA\UiPath Level 2\05 CHALLENGE - Simple enterprise bot\01 Challenge overview NEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\Documents\UiPath\UpdateLeadsCRMBot\LeadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B36EAF-193C-41C0-92DE-B6ABEB717A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2554CC77-060B-485A-99F5-6B104D567567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13350" yWindow="4815" windowWidth="13590" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leads" sheetId="1" r:id="rId1"/>
@@ -324,13 +324,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -640,14 +645,14 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -655,485 +660,485 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>